<commit_message>
Validation terminer + fin de la traduction partie milieu de stage
</commit_message>
<xml_diff>
--- a/Documentation/Echeancier.xlsx
+++ b/Documentation/Echeancier.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adminesp\Documents\InterfaceStages\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierr\Desktop\GestionStages\GestionStages\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F59F2F-1AA2-46CF-9ADA-4AC8676E3AFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="1152" windowWidth="15360" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -71,9 +80,6 @@
     <t>Documentation scolaire + liste des stage vue par l'étudiant</t>
   </si>
   <si>
-    <t>Ordre de préférance des stages de l'étudiant</t>
-  </si>
-  <si>
     <t>Retour sprint 2</t>
   </si>
   <si>
@@ -108,12 +114,15 @@
   </si>
   <si>
     <t>Fin sprint 4</t>
+  </si>
+  <si>
+    <t>Ordre de préférence des stages de l'étudiant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -450,22 +459,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" customWidth="1"/>
     <col min="4" max="4" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>1</f>
         <v>1</v>
@@ -494,7 +503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A4" si="0">A2+1</f>
         <v>2</v>
@@ -509,7 +518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -521,18 +530,18 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>A4+1</f>
         <v>4</v>
@@ -547,13 +556,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>A6+1</f>
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -562,103 +571,103 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>A7+1</f>
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>A9+1</f>
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>A10+1</f>
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>A12+1</f>
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <f>A13+1</f>
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>